<commit_message>
Updated code in payslip, announcement, excel import and announcement
</commit_message>
<xml_diff>
--- a/AttendanceManagement/wwwroot/ExcelTemplates/Volume Master.xlsx
+++ b/AttendanceManagement/wwwroot/ExcelTemplates/Volume Master.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29101"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCDD70CA-EDED-4924-B8EA-4085D716B972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F3F1A82-585D-4581-9023-33ED5116328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>ShortName</t>
   </si>
 </sst>
 </file>
@@ -405,15 +408,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>